<commit_message>
create functions for caching the memory before orthogonalization
</commit_message>
<xml_diff>
--- a/doc/BudgetEstimateGridGeomInC++.xlsx
+++ b/doc/BudgetEstimateGridGeomInC++.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\gridgeom++\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LUCA\ENGINES\GridGeom++\lastCheckout\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3297002C-98D8-4AEA-AB7D-D3B81972B606}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C72FD1B-F8B8-437F-8E25-CD4164E0BC00}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="bestedingen" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -643,7 +643,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>